<commit_message>
fix: downgrade react to 18
</commit_message>
<xml_diff>
--- a/public/base.xlsx
+++ b/public/base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="175">
   <si>
     <t>کارگزاری آینده نگر خوارزمی به مدیریت دکتر ذوقی 09123011311 و 61914000-021 (داخلی 408 الی 411)</t>
   </si>
@@ -673,9 +673,6 @@
 https://t.me/TDI_MDI
 لینک بله⬅️
 ble.ir/join/HLzkvyNxQu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">مقایسه قیمت پاییه پلی وینیل کلراید PVC(S) </t>
   </si>
 </sst>
 </file>
@@ -1202,9 +1199,39 @@
     <xf numFmtId="3" fontId="21" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="21" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1223,21 +1250,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="21" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1248,21 +1260,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2150,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH259"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
@@ -2185,24 +2182,24 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="A2" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
     </row>
     <row r="3" spans="1:34" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="74"/>
+      <c r="A3" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="4" spans="1:34" s="57" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63"/>
@@ -2343,14 +2340,14 @@
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:34" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="68" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="77"/>
     </row>
     <row r="12" spans="1:34" s="24" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="38"/>
@@ -2361,24 +2358,24 @@
       <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
+      <c r="A13" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
     </row>
     <row r="14" spans="1:34" s="57" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="74"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="84"/>
       <c r="G14" s="56"/>
       <c r="H14" s="56"/>
       <c r="I14" s="56"/>
@@ -2579,14 +2576,14 @@
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:34" s="26" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="87"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
@@ -2625,24 +2622,24 @@
       <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:34" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
+      <c r="A26" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
     </row>
     <row r="27" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="74"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="84"/>
     </row>
     <row r="28" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="65"/>
@@ -2726,11 +2723,11 @@
       <c r="A33" s="67" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="88"/>
-      <c r="C33" s="88"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
     </row>
     <row r="34" spans="1:34" s="64" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="38"/>
@@ -2769,24 +2766,24 @@
       <c r="AH34" s="24"/>
     </row>
     <row r="35" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
+      <c r="A35" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
     </row>
     <row r="36" spans="1:34" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="71" t="s">
+      <c r="A36" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="B36" s="72"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="74"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="84"/>
     </row>
     <row r="37" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="65"/>
@@ -3075,14 +3072,14 @@
       <c r="F54" s="31"/>
     </row>
     <row r="55" spans="1:6" s="1" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="76" t="s">
+      <c r="A55" s="68" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="77"/>
-      <c r="C55" s="77"/>
-      <c r="D55" s="77"/>
-      <c r="E55" s="77"/>
-      <c r="F55" s="78"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="70"/>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="38"/>
@@ -3093,20 +3090,20 @@
       <c r="F56" s="31"/>
     </row>
     <row r="57" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="70"/>
-      <c r="C57" s="70"/>
-      <c r="D57" s="70"/>
-      <c r="E57" s="70"/>
-      <c r="F57" s="70"/>
+      <c r="A57" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="80"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="80"/>
     </row>
     <row r="58" spans="1:6" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="79" t="s">
+      <c r="A58" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="B58" s="80"/>
+      <c r="B58" s="85"/>
       <c r="C58" s="75"/>
       <c r="D58" s="75"/>
       <c r="E58" s="75"/>
@@ -3447,14 +3444,14 @@
       <c r="F79" s="31"/>
     </row>
     <row r="80" spans="1:6" s="1" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="76" t="s">
+      <c r="A80" s="68" t="s">
         <v>174</v>
       </c>
-      <c r="B80" s="77"/>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="78"/>
+      <c r="B80" s="69"/>
+      <c r="C80" s="69"/>
+      <c r="D80" s="69"/>
+      <c r="E80" s="69"/>
+      <c r="F80" s="70"/>
     </row>
     <row r="81" spans="1:6" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="38"/>
@@ -3465,24 +3462,24 @@
       <c r="F81" s="31"/>
     </row>
     <row r="82" spans="1:6" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="82"/>
-      <c r="C82" s="82"/>
-      <c r="D82" s="82"/>
-      <c r="E82" s="82"/>
-      <c r="F82" s="83"/>
+      <c r="A82" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="87"/>
+      <c r="C82" s="87"/>
+      <c r="D82" s="87"/>
+      <c r="E82" s="87"/>
+      <c r="F82" s="88"/>
     </row>
     <row r="83" spans="1:6" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="79" t="s">
+      <c r="A83" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="84"/>
-      <c r="C83" s="85"/>
-      <c r="D83" s="85"/>
-      <c r="E83" s="85"/>
-      <c r="F83" s="85"/>
+      <c r="B83" s="73"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+      <c r="F83" s="74"/>
     </row>
     <row r="84" spans="1:6" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="61"/>
@@ -3783,14 +3780,14 @@
       <c r="F100" s="31"/>
     </row>
     <row r="101" spans="1:34" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="76" t="s">
+      <c r="A101" s="68" t="s">
         <v>167</v>
       </c>
-      <c r="B101" s="77"/>
-      <c r="C101" s="77"/>
-      <c r="D101" s="77"/>
-      <c r="E101" s="77"/>
-      <c r="F101" s="78"/>
+      <c r="B101" s="69"/>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="70"/>
     </row>
     <row r="102" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="38"/>
@@ -3811,14 +3808,14 @@
       <c r="F103" s="75"/>
     </row>
     <row r="104" spans="1:34" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="79" t="s">
+      <c r="A104" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="84"/>
-      <c r="C104" s="85"/>
-      <c r="D104" s="85"/>
-      <c r="E104" s="85"/>
-      <c r="F104" s="85"/>
+      <c r="B104" s="73"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="74"/>
     </row>
     <row r="105" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="61"/>
@@ -4087,14 +4084,14 @@
       <c r="F119" s="24"/>
     </row>
     <row r="120" spans="1:34" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="76" t="s">
+      <c r="A120" s="68" t="s">
         <v>168</v>
       </c>
-      <c r="B120" s="77"/>
-      <c r="C120" s="77"/>
-      <c r="D120" s="77"/>
-      <c r="E120" s="77"/>
-      <c r="F120" s="78"/>
+      <c r="B120" s="69"/>
+      <c r="C120" s="69"/>
+      <c r="D120" s="69"/>
+      <c r="E120" s="69"/>
+      <c r="F120" s="70"/>
     </row>
     <row r="121" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="36"/>
@@ -4115,14 +4112,14 @@
       <c r="F122" s="75"/>
     </row>
     <row r="123" spans="1:34" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="79" t="s">
+      <c r="A123" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="B123" s="84"/>
-      <c r="C123" s="85"/>
-      <c r="D123" s="85"/>
-      <c r="E123" s="85"/>
-      <c r="F123" s="85"/>
+      <c r="B123" s="73"/>
+      <c r="C123" s="74"/>
+      <c r="D123" s="74"/>
+      <c r="E123" s="74"/>
+      <c r="F123" s="74"/>
     </row>
     <row r="124" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="61"/>
@@ -4355,14 +4352,14 @@
       <c r="F134" s="37"/>
     </row>
     <row r="135" spans="1:34" ht="147" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="76" t="s">
+      <c r="A135" s="68" t="s">
         <v>169</v>
       </c>
-      <c r="B135" s="77"/>
-      <c r="C135" s="77"/>
-      <c r="D135" s="77"/>
-      <c r="E135" s="77"/>
-      <c r="F135" s="78"/>
+      <c r="B135" s="69"/>
+      <c r="C135" s="69"/>
+      <c r="D135" s="69"/>
+      <c r="E135" s="69"/>
+      <c r="F135" s="70"/>
     </row>
     <row r="136" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="36"/>
@@ -4383,14 +4380,14 @@
       <c r="F137" s="75"/>
     </row>
     <row r="138" spans="1:34" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="79" t="s">
+      <c r="A138" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="B138" s="84"/>
-      <c r="C138" s="85"/>
-      <c r="D138" s="85"/>
-      <c r="E138" s="85"/>
-      <c r="F138" s="85"/>
+      <c r="B138" s="73"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="74"/>
+      <c r="F138" s="74"/>
     </row>
     <row r="139" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="61"/>
@@ -4579,14 +4576,14 @@
       <c r="F148" s="24"/>
     </row>
     <row r="149" spans="1:6" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="76" t="s">
+      <c r="A149" s="68" t="s">
         <v>170</v>
       </c>
-      <c r="B149" s="77"/>
-      <c r="C149" s="77"/>
-      <c r="D149" s="77"/>
-      <c r="E149" s="77"/>
-      <c r="F149" s="78"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="69"/>
+      <c r="D149" s="69"/>
+      <c r="E149" s="69"/>
+      <c r="F149" s="70"/>
     </row>
     <row r="150" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="36"/>
@@ -4607,14 +4604,14 @@
       <c r="F151" s="75"/>
     </row>
     <row r="152" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="84" t="s">
+      <c r="A152" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="B152" s="84"/>
-      <c r="C152" s="85"/>
-      <c r="D152" s="85"/>
-      <c r="E152" s="85"/>
-      <c r="F152" s="85"/>
+      <c r="B152" s="73"/>
+      <c r="C152" s="74"/>
+      <c r="D152" s="74"/>
+      <c r="E152" s="74"/>
+      <c r="F152" s="74"/>
     </row>
     <row r="153" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="61"/>
@@ -5018,11 +5015,11 @@
       <c r="A178" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="B178" s="68"/>
-      <c r="C178" s="68"/>
-      <c r="D178" s="68"/>
-      <c r="E178" s="68"/>
-      <c r="F178" s="68"/>
+      <c r="B178" s="71"/>
+      <c r="C178" s="71"/>
+      <c r="D178" s="71"/>
+      <c r="E178" s="71"/>
+      <c r="F178" s="71"/>
     </row>
     <row r="179" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="36"/>
@@ -5043,14 +5040,14 @@
       <c r="F180" s="75"/>
     </row>
     <row r="181" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="79" t="s">
+      <c r="A181" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="B181" s="84"/>
-      <c r="C181" s="85"/>
-      <c r="D181" s="85"/>
-      <c r="E181" s="85"/>
-      <c r="F181" s="85"/>
+      <c r="B181" s="73"/>
+      <c r="C181" s="74"/>
+      <c r="D181" s="74"/>
+      <c r="E181" s="74"/>
+      <c r="F181" s="74"/>
     </row>
     <row r="182" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="61"/>
@@ -5466,11 +5463,11 @@
       <c r="A206" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="B206" s="68"/>
-      <c r="C206" s="68"/>
-      <c r="D206" s="68"/>
-      <c r="E206" s="68"/>
-      <c r="F206" s="68"/>
+      <c r="B206" s="71"/>
+      <c r="C206" s="71"/>
+      <c r="D206" s="71"/>
+      <c r="E206" s="71"/>
+      <c r="F206" s="71"/>
     </row>
     <row r="207" spans="1:34" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="36"/>
@@ -5491,14 +5488,14 @@
       <c r="F208" s="75"/>
     </row>
     <row r="209" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="79" t="s">
+      <c r="A209" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="B209" s="84"/>
-      <c r="C209" s="85"/>
-      <c r="D209" s="85"/>
-      <c r="E209" s="85"/>
-      <c r="F209" s="85"/>
+      <c r="B209" s="73"/>
+      <c r="C209" s="74"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
+      <c r="F209" s="74"/>
     </row>
     <row r="210" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="61"/>
@@ -5598,11 +5595,11 @@
       <c r="A216" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="B216" s="68"/>
-      <c r="C216" s="68"/>
-      <c r="D216" s="68"/>
-      <c r="E216" s="68"/>
-      <c r="F216" s="68"/>
+      <c r="B216" s="71"/>
+      <c r="C216" s="71"/>
+      <c r="D216" s="71"/>
+      <c r="E216" s="71"/>
+      <c r="F216" s="71"/>
     </row>
     <row r="217" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="58"/>
@@ -5623,14 +5620,14 @@
       <c r="F218" s="75"/>
     </row>
     <row r="219" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="79" t="s">
+      <c r="A219" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="B219" s="84"/>
-      <c r="C219" s="85"/>
-      <c r="D219" s="85"/>
-      <c r="E219" s="85"/>
-      <c r="F219" s="85"/>
+      <c r="B219" s="73"/>
+      <c r="C219" s="74"/>
+      <c r="D219" s="74"/>
+      <c r="E219" s="74"/>
+      <c r="F219" s="74"/>
     </row>
     <row r="220" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="61"/>
@@ -6264,6 +6261,29 @@
     <sortCondition ref="B131"/>
   </sortState>
   <mergeCells count="39">
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A151:F151"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="A103:F103"/>
+    <mergeCell ref="A104:F104"/>
+    <mergeCell ref="A122:F122"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A101:F101"/>
     <mergeCell ref="A259:F259"/>
     <mergeCell ref="A120:F120"/>
     <mergeCell ref="A135:F135"/>
@@ -6280,29 +6300,6 @@
     <mergeCell ref="A180:F180"/>
     <mergeCell ref="A181:F181"/>
     <mergeCell ref="A208:F208"/>
-    <mergeCell ref="A104:F104"/>
-    <mergeCell ref="A122:F122"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A101:F101"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A151:F151"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A55:F55"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="A103:F103"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6334,11 +6331,11 @@
       <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
     </row>
     <row r="2" spans="1:6" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="89" t="s">

</xml_diff>